<commit_message>
Design changes Alignment and extra code removed
</commit_message>
<xml_diff>
--- a/src/main/resources/nxData_prod.xlsx
+++ b/src/main/resources/nxData_prod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MunishData\mp\project\workspace\shop\shop\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MunishData\mp\nxdial\nxdial\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1801AF47-6D72-435D-AF27-B8A0DAF62AB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D8ECBB-0D8F-4F9F-9516-EA2A6B80B218}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="11" activeTab="14" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="24" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5328" uniqueCount="2475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5329" uniqueCount="2476">
   <si>
     <t>RESTAURANTS</t>
   </si>
@@ -7573,6 +7573,9 @@
   </si>
   <si>
     <t>08650100534</t>
+  </si>
+  <si>
+    <t>The UP government cleared the decks for the expansion of the metro network to Noida Extension</t>
   </si>
 </sst>
 </file>
@@ -15486,7 +15489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148CF0CC-1380-4358-9D85-83EE3B667E76}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -23023,8 +23026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6423CCE-6EB8-4EF2-8139-9A238685283D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23051,11 +23054,9 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2299</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>2298</v>
-      </c>
+        <v>2475</v>
+      </c>
+      <c r="B3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23065,10 +23066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5551A84-3C39-4D9D-A279-933A50692AE3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23091,6 +23092,14 @@
       </c>
       <c r="B2" s="7" t="s">
         <v>876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>